<commit_message>
klar itl å reise hjem
</commit_message>
<xml_diff>
--- a/Kalkulasjoner.xlsx
+++ b/Kalkulasjoner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oyste\Documents\Masteroppgave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oystmol\Documents\Masteroppgave\Ting fra hjemme 2\masteren\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7961748D-11F4-495B-BFD2-5098069CCAAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18F3880-15B8-40A4-AB31-3D2BC6F23F5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A1B7EC4E-B536-4F30-A5EA-E8C07AF799B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A1B7EC4E-B536-4F30-A5EA-E8C07AF799B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -506,12 +504,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -520,6 +512,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -838,79 +836,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4646F704-F7EC-4153-B4A6-AAFFBD6E7FF7}">
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="3" width="9.109375" style="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="19" max="19" width="11.109375" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="28"/>
+      <c r="K4" s="30"/>
       <c r="L4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="28" t="s">
+      <c r="N4" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="28"/>
+      <c r="O4" s="30"/>
       <c r="P4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="28" t="s">
+      <c r="R4" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="S4" s="28"/>
+      <c r="S4" s="30"/>
       <c r="T4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -927,16 +925,16 @@
       <c r="G5">
         <v>50</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="31">
         <v>0.05</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="31" t="s">
         <v>17</v>
       </c>
       <c r="N5" t="s">
@@ -946,7 +944,7 @@
         <f>Vdd*1000/G_F</f>
         <v>66</v>
       </c>
-      <c r="P5" s="27" t="s">
+      <c r="P5" s="31" t="s">
         <v>15</v>
       </c>
       <c r="R5" t="s">
@@ -955,11 +953,11 @@
       <c r="S5">
         <v>2</v>
       </c>
-      <c r="T5" s="27" t="s">
+      <c r="T5" s="31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
@@ -975,10 +973,10 @@
       <c r="G6">
         <v>100</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
+      <c r="H6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
       <c r="N6" t="s">
         <v>12</v>
       </c>
@@ -986,16 +984,16 @@
         <f>Vdd*1000/G_H</f>
         <v>33</v>
       </c>
-      <c r="P6" s="27"/>
+      <c r="P6" s="31"/>
       <c r="R6" t="s">
         <v>27</v>
       </c>
       <c r="S6">
         <v>2</v>
       </c>
-      <c r="T6" s="27"/>
-    </row>
-    <row r="7" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+      <c r="T6" s="31"/>
+    </row>
+    <row r="7" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>39</v>
       </c>
@@ -1011,10 +1009,10 @@
       <c r="G7">
         <v>200</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+      <c r="H7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
       <c r="N7" t="s">
         <v>13</v>
       </c>
@@ -1022,26 +1020,26 @@
         <f>Vdd*1000/G_W</f>
         <v>16.5</v>
       </c>
-      <c r="P7" s="27"/>
+      <c r="P7" s="31"/>
       <c r="R7" t="s">
         <v>28</v>
       </c>
       <c r="S7">
         <v>10</v>
       </c>
-      <c r="T7" s="27"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="T7" s="31"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>8</v>
       </c>
       <c r="G8">
         <v>500</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
+      <c r="H8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
       <c r="N8" t="s">
         <v>14</v>
       </c>
@@ -1049,51 +1047,51 @@
         <f>Vdd*1000/G_E</f>
         <v>6.6</v>
       </c>
-      <c r="P8" s="27"/>
+      <c r="P8" s="31"/>
       <c r="R8" t="s">
         <v>29</v>
       </c>
       <c r="S8">
         <v>15</v>
       </c>
-      <c r="T8" s="27"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="T8" s="31"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="E10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="I10" s="28"/>
+      <c r="I10" s="30"/>
       <c r="J10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="L10" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="M10" s="28"/>
+      <c r="M10" s="30"/>
       <c r="N10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P10" s="30" t="s">
+      <c r="P10" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="W10" s="29" t="s">
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="W10" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1110,7 +1108,7 @@
         <f>FLOOR(V_s_F/I_max,0.01)</f>
         <v>0.18</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="31" t="s">
         <v>58</v>
       </c>
       <c r="L11" t="s">
@@ -1120,14 +1118,14 @@
         <f>FLOOR(V_s_F/I_max2,0.01)</f>
         <v>0.2</v>
       </c>
-      <c r="N11" s="27" t="s">
+      <c r="N11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="W11" s="29"/>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="29"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1143,7 +1141,7 @@
         <f>(C12-B12)/2</f>
         <v>1.4851000000003296</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="31" t="s">
         <v>15</v>
       </c>
       <c r="H12" t="s">
@@ -1153,7 +1151,7 @@
         <f>V_s_H/I_max</f>
         <v>9.4285714285714292E-2</v>
       </c>
-      <c r="J12" s="27"/>
+      <c r="J12" s="31"/>
       <c r="L12" t="s">
         <v>34</v>
       </c>
@@ -1161,7 +1159,7 @@
         <f>V_s_H/I_max2</f>
         <v>0.1</v>
       </c>
-      <c r="N12" s="27"/>
+      <c r="N12" s="31"/>
       <c r="P12" t="s">
         <v>65</v>
       </c>
@@ -1182,7 +1180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>20</v>
       </c>
@@ -1198,7 +1196,7 @@
         <f t="shared" ref="D13:D15" si="0">(C13-B13)/2</f>
         <v>1.6502000000000407</v>
       </c>
-      <c r="E13" s="27"/>
+      <c r="E13" s="31"/>
       <c r="H13" t="s">
         <v>35</v>
       </c>
@@ -1206,7 +1204,7 @@
         <f>V_s_W/I_max</f>
         <v>4.7142857142857146E-2</v>
       </c>
-      <c r="J13" s="27"/>
+      <c r="J13" s="31"/>
       <c r="L13" t="s">
         <v>35</v>
       </c>
@@ -1214,7 +1212,7 @@
         <f>V_s_W/I_max2</f>
         <v>0.05</v>
       </c>
-      <c r="N13" s="27"/>
+      <c r="N13" s="31"/>
       <c r="P13" t="s">
         <v>66</v>
       </c>
@@ -1232,7 +1230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>21</v>
       </c>
@@ -1248,7 +1246,7 @@
         <f t="shared" si="0"/>
         <v>1.6520000000000437</v>
       </c>
-      <c r="E14" s="27"/>
+      <c r="E14" s="31"/>
       <c r="H14" t="s">
         <v>36</v>
       </c>
@@ -1256,7 +1254,7 @@
         <f>V_s_E/I_max</f>
         <v>1.8857142857142857E-2</v>
       </c>
-      <c r="J14" s="27"/>
+      <c r="J14" s="31"/>
       <c r="L14" t="s">
         <v>36</v>
       </c>
@@ -1264,7 +1262,7 @@
         <f>V_s_E/I_max2</f>
         <v>0.02</v>
       </c>
-      <c r="N14" s="27"/>
+      <c r="N14" s="31"/>
       <c r="W14" t="s">
         <v>59</v>
       </c>
@@ -1275,7 +1273,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>22</v>
       </c>
@@ -1291,7 +1289,7 @@
         <f t="shared" si="0"/>
         <v>1.6575000000000273</v>
       </c>
-      <c r="E15" s="27"/>
+      <c r="E15" s="31"/>
       <c r="W15" s="19" t="s">
         <v>62</v>
       </c>
@@ -1303,7 +1301,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
         <v>67</v>
       </c>
@@ -1323,7 +1321,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="W17" t="s">
         <v>84</v>
       </c>
@@ -1334,21 +1332,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" s="31" t="s">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="J18" s="31" t="s">
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="J18" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
       <c r="W18" t="s">
         <v>59</v>
       </c>
@@ -1359,17 +1357,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
       <c r="W19" t="s">
         <v>62</v>
       </c>
@@ -1380,17 +1378,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
       <c r="W20" s="19" t="s">
         <v>60</v>
       </c>
@@ -1399,19 +1397,19 @@
         <v>3.2949790794979084</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="10" t="s">
         <v>47</v>
@@ -1445,7 +1443,7 @@
       <c r="S22" s="9"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>42</v>
       </c>
@@ -1483,7 +1481,7 @@
       <c r="S23" s="9"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>41</v>
       </c>
@@ -1521,7 +1519,7 @@
       <c r="S24" s="9"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>45</v>
       </c>
@@ -1557,7 +1555,7 @@
       <c r="S25" s="9"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>50</v>
       </c>
@@ -1599,7 +1597,7 @@
       <c r="S26" s="9"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1619,7 +1617,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -1645,7 +1643,7 @@
       <c r="S28" s="9"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>52</v>
       </c>
@@ -1681,7 +1679,7 @@
       <c r="S29" s="9"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>53</v>
       </c>
@@ -1715,7 +1713,7 @@
       <c r="S30" s="9"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>55</v>
       </c>
@@ -1753,7 +1751,7 @@
       <c r="S31" s="9"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>56</v>
       </c>
@@ -1782,7 +1780,7 @@
       <c r="S32" s="9"/>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>57</v>
       </c>
@@ -1811,7 +1809,7 @@
       <c r="S33" s="9"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1833,7 +1831,7 @@
       <c r="S34" s="9"/>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>77</v>
       </c>
@@ -1863,7 +1861,7 @@
       <c r="S35" s="9"/>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>80</v>
       </c>
@@ -1893,7 +1891,7 @@
       <c r="S36" s="9"/>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>81</v>
       </c>
@@ -1914,7 +1912,7 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
       <c r="M38" s="16"/>
@@ -1925,7 +1923,7 @@
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1946,7 +1944,7 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -1971,7 +1969,7 @@
       <c r="Y40" s="9"/>
       <c r="Z40" s="9"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1997,7 +1995,7 @@
       <c r="Y41" s="9"/>
       <c r="Z41" s="9"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -2018,7 +2016,7 @@
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
     </row>
-    <row r="43" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="43" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
@@ -2039,7 +2037,7 @@
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
     </row>
-    <row r="44" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="44" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A44" s="21"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
@@ -2060,7 +2058,7 @@
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
     </row>
-    <row r="45" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="45" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A45" s="21"/>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
@@ -2081,7 +2079,7 @@
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
     </row>
-    <row r="46" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="46" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A46" s="21"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -2102,7 +2100,7 @@
       <c r="R46" s="8"/>
       <c r="S46" s="8"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -2120,7 +2118,7 @@
       <c r="O47" s="9"/>
       <c r="P47" s="8"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
@@ -2136,7 +2134,7 @@
       <c r="O48" s="9"/>
       <c r="P48" s="8"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -2154,7 +2152,7 @@
       <c r="O49" s="9"/>
       <c r="P49" s="8"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -2172,7 +2170,7 @@
       <c r="O50" s="9"/>
       <c r="P50" s="8"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="20"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
@@ -2189,7 +2187,7 @@
       <c r="O51" s="9"/>
       <c r="P51" s="8"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
@@ -2204,7 +2202,7 @@
       <c r="O52" s="9"/>
       <c r="P52" s="8"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
@@ -2219,7 +2217,7 @@
       <c r="O53" s="9"/>
       <c r="P53" s="8"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -2237,7 +2235,7 @@
       <c r="O54" s="8"/>
       <c r="P54" s="8"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -2255,7 +2253,7 @@
       <c r="O55" s="8"/>
       <c r="P55" s="8"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -2273,7 +2271,7 @@
       <c r="O56" s="8"/>
       <c r="P56" s="8"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -2291,7 +2289,7 @@
       <c r="O57" s="8"/>
       <c r="P57" s="8"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -2309,7 +2307,7 @@
       <c r="O58" s="8"/>
       <c r="P58" s="8"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -2327,7 +2325,7 @@
       <c r="O59" s="8"/>
       <c r="P59" s="8"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -2345,7 +2343,7 @@
       <c r="O60" s="8"/>
       <c r="P60" s="8"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -2365,6 +2363,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J11:J14"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N11:N14"/>
     <mergeCell ref="W10:Y11"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="A18:E21"/>
@@ -2381,11 +2384,6 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="R4:S4"/>
     <mergeCell ref="T5:T8"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J11:J14"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N11:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>